<commit_message>
NLC 2026: update export data, fix name display, seed 454 registrants
- Update export source to Export-20260219 (271 sign-ups)
- Add spouse/companion name resolution in relate_nlc_export.py: infers
  last name for rows with no Flocknote ID and same confirmation number
- Fix seed _normalizeKey to strip apostrophes so "Person's Name" columns
  map correctly to profile.firstName / profile.lastName (was showing "?")
- Seed: 454 registrants, 266 session pre-registrations
- Update firestore.rules: allow delete/create on registrants and
  sessionRegistrations for nlc-2026 (seed tool support)
- Add docs/data2/summary_count.md with full reconciliation details
- Clean up demo.md stats section with current counts

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/docs/data2/Sessions_matched_to_nlc_registraion.xlsx
+++ b/docs/data2/Sessions_matched_to_nlc_registraion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aisaiah/Documents/users/aisaiah/aisaiah_workspace/flutter/event-hub/docs/data2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ABF39BE2-8C60-944A-BE18-24AC5D320581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86711AC5-B37F-FB42-B0F6-5A86AE616804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69200" yWindow="1960" windowWidth="45420" windowHeight="22140" activeTab="1" xr2:uid="{43511E8B-4281-0F4E-A31B-8AEE10E81452}"/>
+    <workbookView xWindow="59300" yWindow="5920" windowWidth="45420" windowHeight="22140" activeTab="2" xr2:uid="{43511E8B-4281-0F4E-A31B-8AEE10E81452}"/>
   </bookViews>
   <sheets>
     <sheet name="Session_NOT_matched_to_nlc_reg" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="nlc_registration" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">nlc_registration!$A$1:$AM$457</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Session_matched_to_nlc_reg!$A$1:$N$248</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -10118,7 +10119,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10245,8 +10246,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="C1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="F197" sqref="F197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12141,7 +12142,7 @@
         <v>capecharles8@gmail.com</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>218</v>
       </c>
@@ -12182,7 +12183,7 @@
         <v>cocoyusa049@gmail.com</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>218</v>
       </c>
@@ -12551,7 +12552,7 @@
         <v>THECOROOKS@GMAIL.COM</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>265</v>
       </c>
@@ -14577,7 +14578,7 @@
         <v>annlucero30@gmail.com</v>
       </c>
     </row>
-    <row r="107" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>485</v>
       </c>
@@ -15101,7 +15102,7 @@
         <v>goemailalvin@gmail.com</v>
       </c>
     </row>
-    <row r="120" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>542</v>
       </c>
@@ -17745,7 +17746,7 @@
         <v>rubyvegafria67@yahoo.com</v>
       </c>
     </row>
-    <row r="185" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>822</v>
       </c>
@@ -18114,7 +18115,7 @@
         <v>amiazaide@gmail.com</v>
       </c>
     </row>
-    <row r="194" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>863</v>
       </c>
@@ -18155,7 +18156,7 @@
         <v>alazasrebecca@gmail.com</v>
       </c>
     </row>
-    <row r="195" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>868</v>
       </c>
@@ -18196,7 +18197,7 @@
         <v>cfcarnelarce@yahoo.com</v>
       </c>
     </row>
-    <row r="196" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>874</v>
       </c>
@@ -18278,7 +18279,7 @@
         <v>pjbanzon@yahoo.com</v>
       </c>
     </row>
-    <row r="198" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>883</v>
       </c>
@@ -18319,7 +18320,7 @@
         <v>armandodc2023@gmail.com</v>
       </c>
     </row>
-    <row r="199" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>888</v>
       </c>
@@ -18360,7 +18361,7 @@
         <v>monoma@att.net</v>
       </c>
     </row>
-    <row r="200" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>893</v>
       </c>
@@ -18401,7 +18402,7 @@
         <v>nesreyesdimac@gmail.com</v>
       </c>
     </row>
-    <row r="201" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
         <v>898</v>
       </c>
@@ -18442,7 +18443,7 @@
         <v>rc.estrera@gmail.com</v>
       </c>
     </row>
-    <row r="202" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>902</v>
       </c>
@@ -18483,7 +18484,7 @@
         <v>james.francisco@couplesforchristusa.org</v>
       </c>
     </row>
-    <row r="203" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
         <v>907</v>
       </c>
@@ -18524,7 +18525,7 @@
         <v>eggaymadelgonda@gmail.com</v>
       </c>
     </row>
-    <row r="204" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>912</v>
       </c>
@@ -18565,7 +18566,7 @@
         <v>bochoc@gmail.com</v>
       </c>
     </row>
-    <row r="205" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>915</v>
       </c>
@@ -18606,7 +18607,7 @@
         <v>lynnette.guirao@gmail.com</v>
       </c>
     </row>
-    <row r="206" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>920</v>
       </c>
@@ -18644,7 +18645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>922</v>
       </c>
@@ -18685,7 +18686,7 @@
         <v>4crux68@gmail.com</v>
       </c>
     </row>
-    <row r="208" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>927</v>
       </c>
@@ -18726,7 +18727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
         <v>932</v>
       </c>
@@ -18767,7 +18768,7 @@
         <v>rmlapitan229@gmail.com</v>
       </c>
     </row>
-    <row r="210" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
         <v>937</v>
       </c>
@@ -18808,7 +18809,7 @@
         <v>arnoldlim2006@yahoo.com</v>
       </c>
     </row>
-    <row r="211" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
         <v>941</v>
       </c>
@@ -18849,7 +18850,7 @@
         <v>judith_lladoc@yahoo.com</v>
       </c>
     </row>
-    <row r="212" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>944</v>
       </c>
@@ -18890,7 +18891,7 @@
         <v>afo.magat@gmail.com</v>
       </c>
     </row>
-    <row r="213" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
         <v>948</v>
       </c>
@@ -18931,7 +18932,7 @@
         <v>jsmalins19@msn.com</v>
       </c>
     </row>
-    <row r="214" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>952</v>
       </c>
@@ -18972,7 +18973,7 @@
         <v>manuelgmarcelino@yahoo.com</v>
       </c>
     </row>
-    <row r="215" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>956</v>
       </c>
@@ -19013,7 +19014,7 @@
         <v>cfchercules@gmail.com</v>
       </c>
     </row>
-    <row r="216" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>960</v>
       </c>
@@ -19054,7 +19055,7 @@
         <v>pablitomelgarejojr@gmail.com</v>
       </c>
     </row>
-    <row r="217" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
         <v>965</v>
       </c>
@@ -19095,7 +19096,7 @@
         <v>BOBBEE.CFC@GMAIL.COM</v>
       </c>
     </row>
-    <row r="218" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
         <v>970</v>
       </c>
@@ -19133,7 +19134,7 @@
         <v>marivic.cfc92@gmail.com</v>
       </c>
     </row>
-    <row r="219" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
         <v>972</v>
       </c>
@@ -19174,7 +19175,7 @@
         <v>mirandlo@gmail.com</v>
       </c>
     </row>
-    <row r="220" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
         <v>976</v>
       </c>
@@ -19215,7 +19216,7 @@
         <v>rcmirano@prodigy.net</v>
       </c>
     </row>
-    <row r="221" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="4" t="s">
         <v>981</v>
       </c>
@@ -19256,7 +19257,7 @@
         <v>junnapuli1234@gmail.com</v>
       </c>
     </row>
-    <row r="222" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
         <v>986</v>
       </c>
@@ -19297,7 +19298,7 @@
         <v>jnj_olalia@yahoo.com</v>
       </c>
     </row>
-    <row r="223" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
         <v>991</v>
       </c>
@@ -19338,7 +19339,7 @@
         <v>peterluong120@gmail.com</v>
       </c>
     </row>
-    <row r="224" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>996</v>
       </c>
@@ -19379,7 +19380,7 @@
         <v>joeeleanor@yahoo.com</v>
       </c>
     </row>
-    <row r="225" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
         <v>1001</v>
       </c>
@@ -19420,7 +19421,7 @@
         <v>rey.reyes711@gmail.com</v>
       </c>
     </row>
-    <row r="226" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
         <v>1006</v>
       </c>
@@ -19461,7 +19462,7 @@
         <v>arturorg11@hotmail.com</v>
       </c>
     </row>
-    <row r="227" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="4" t="s">
         <v>1011</v>
       </c>
@@ -19502,7 +19503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="4" t="s">
         <v>1016</v>
       </c>
@@ -19543,7 +19544,7 @@
         <v>emilsarm@aol.com</v>
       </c>
     </row>
-    <row r="229" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="4" t="s">
         <v>1021</v>
       </c>
@@ -19584,7 +19585,7 @@
         <v>sherreff@gmail.com</v>
       </c>
     </row>
-    <row r="230" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
         <v>1025</v>
       </c>
@@ -19625,7 +19626,7 @@
         <v>jsicam72@gmail.com</v>
       </c>
     </row>
-    <row r="231" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
         <v>1029</v>
       </c>
@@ -19666,7 +19667,7 @@
         <v>dave.sliter@hotmail.com</v>
       </c>
     </row>
-    <row r="232" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
         <v>1033</v>
       </c>
@@ -19707,7 +19708,7 @@
         <v>chipstenoso@yahoo.com</v>
       </c>
     </row>
-    <row r="233" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>1038</v>
       </c>
@@ -19748,7 +19749,7 @@
         <v>froylantoledo@yahoo.com</v>
       </c>
     </row>
-    <row r="234" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>1043</v>
       </c>
@@ -19786,7 +19787,7 @@
         <v>adeline.toledo@gmail.com</v>
       </c>
     </row>
-    <row r="235" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
         <v>1045</v>
       </c>
@@ -19827,7 +19828,7 @@
         <v>emvegafria@yahoo.com</v>
       </c>
     </row>
-    <row r="236" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
         <v>1050</v>
       </c>
@@ -19868,7 +19869,7 @@
         <v>dinoworx@yahoo.com</v>
       </c>
     </row>
-    <row r="237" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
         <v>1054</v>
       </c>
@@ -19909,7 +19910,7 @@
         <v>emmanuelzaide1@gmail.com</v>
       </c>
     </row>
-    <row r="238" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
         <v>1059</v>
       </c>
@@ -19944,7 +19945,7 @@
         <v>gigialcaraz@yahoo.com</v>
       </c>
     </row>
-    <row r="239" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
         <v>1061</v>
       </c>
@@ -19979,7 +19980,7 @@
         <v>arthur.gutierrez@yahoo.com</v>
       </c>
     </row>
-    <row r="240" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>1063</v>
       </c>
@@ -20014,7 +20015,7 @@
         <v>maryann.gutierrez@yahoo.com</v>
       </c>
     </row>
-    <row r="241" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
         <v>1065</v>
       </c>
@@ -20049,7 +20050,7 @@
         <v>fondevsp@gmail.com</v>
       </c>
     </row>
-    <row r="242" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
         <v>1067</v>
       </c>
@@ -20084,7 +20085,7 @@
         <v>Minniemalibiran26.2@gmail.com</v>
       </c>
     </row>
-    <row r="243" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="4" t="s">
         <v>1069</v>
       </c>
@@ -20119,7 +20120,7 @@
         <v>vickydperalta@gmail.com</v>
       </c>
     </row>
-    <row r="244" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
         <v>1071</v>
       </c>
@@ -20157,7 +20158,7 @@
         <v>rmlapitan229@gmail.com</v>
       </c>
     </row>
-    <row r="245" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="4" t="s">
         <v>1074</v>
       </c>
@@ -20198,7 +20199,7 @@
         <v>arvie.lacson@couplesforchristusa.org</v>
       </c>
     </row>
-    <row r="246" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
         <v>1077</v>
       </c>
@@ -20239,7 +20240,7 @@
         <v>inigo.arcadio@yahoo.com</v>
       </c>
     </row>
-    <row r="247" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
         <v>1082</v>
       </c>
@@ -20280,7 +20281,7 @@
         <v>usafdevega@yahoo.com</v>
       </c>
     </row>
-    <row r="248" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>1087</v>
       </c>
@@ -20326,6 +20327,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="possible_match"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="B76W4"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -20335,10 +20341,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FE1BF5-4620-9740-887F-71B14DF2DAE5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AM457"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G468" sqref="G468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20466,7 +20473,7 @@
         <v>3012</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3011</v>
       </c>
@@ -20483,7 +20490,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3009</v>
       </c>
@@ -20500,7 +20507,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3007</v>
       </c>
@@ -20517,7 +20524,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3005</v>
       </c>
@@ -20534,7 +20541,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3003</v>
       </c>
@@ -20551,7 +20558,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3000</v>
       </c>
@@ -20604,7 +20611,7 @@
         <v>2995</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2997</v>
       </c>
@@ -20657,7 +20664,7 @@
         <v>2995</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2994</v>
       </c>
@@ -20674,7 +20681,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2993</v>
       </c>
@@ -20691,7 +20698,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1011</v>
       </c>
@@ -20732,7 +20739,7 @@
         <v>46069.994444444441</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2989</v>
       </c>
@@ -20749,7 +20756,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>628</v>
       </c>
@@ -20790,7 +20797,7 @@
         <v>46058.80972222222</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2985</v>
       </c>
@@ -20807,7 +20814,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>920</v>
       </c>
@@ -20845,7 +20852,7 @@
         <v>46069.470138888886</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>403</v>
       </c>
@@ -20886,7 +20893,7 @@
         <v>46069.470138888886</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2982</v>
       </c>
@@ -20906,7 +20913,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2979</v>
       </c>
@@ -20926,7 +20933,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2975</v>
       </c>
@@ -20946,7 +20953,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2972</v>
       </c>
@@ -20966,7 +20973,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2968</v>
       </c>
@@ -21016,7 +21023,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2965</v>
       </c>
@@ -21066,7 +21073,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2963</v>
       </c>
@@ -21116,7 +21123,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>360</v>
       </c>
@@ -21190,7 +21197,7 @@
         <v>46070.795138888891</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>365</v>
       </c>
@@ -21264,7 +21271,7 @@
         <v>46064.900694444441</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2960</v>
       </c>
@@ -21314,7 +21321,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2959</v>
       </c>
@@ -21364,7 +21371,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2957</v>
       </c>
@@ -21414,7 +21421,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2955</v>
       </c>
@@ -21464,7 +21471,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>927</v>
       </c>
@@ -21538,7 +21545,7 @@
         <v>46056.347222222219</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2951</v>
       </c>
@@ -21588,7 +21595,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2948</v>
       </c>
@@ -21641,7 +21648,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2946</v>
       </c>
@@ -21694,7 +21701,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2942</v>
       </c>
@@ -21747,7 +21754,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2940</v>
       </c>
@@ -21800,7 +21807,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2936</v>
       </c>
@@ -21853,7 +21860,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>2934</v>
       </c>
@@ -21906,7 +21913,7 @@
         <v>2930</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>247</v>
       </c>
@@ -22007,7 +22014,7 @@
         <v>46067.459027777775</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>252</v>
       </c>
@@ -22108,7 +22115,7 @@
         <v>46064.838194444441</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2921</v>
       </c>
@@ -22185,7 +22192,7 @@
         <v>46057.586458333331</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>2919</v>
       </c>
@@ -22262,7 +22269,7 @@
         <v>46057.586458333331</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2912</v>
       </c>
@@ -22333,7 +22340,7 @@
         <v>46057.584456018521</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>2908</v>
       </c>
@@ -22407,7 +22414,7 @@
         <v>46056.43476851852</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>2906</v>
       </c>
@@ -22481,7 +22488,7 @@
         <v>46056.43476851852</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>2901</v>
       </c>
@@ -22552,7 +22559,7 @@
         <v>46056.430138888885</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>2897</v>
       </c>
@@ -22623,7 +22630,7 @@
         <v>46056.430138888885</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2890</v>
       </c>
@@ -22697,7 +22704,7 @@
         <v>46056.423703703702</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>713</v>
       </c>
@@ -22795,7 +22802,7 @@
         <v>46058.802777777775</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>722</v>
       </c>
@@ -22893,7 +22900,7 @@
         <v>46058.802083333336</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>2875</v>
       </c>
@@ -22967,7 +22974,7 @@
         <v>46056.011400462965</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>2873</v>
       </c>
@@ -23044,7 +23051,7 @@
         <v>46056.011400462965</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>2864</v>
       </c>
@@ -23115,7 +23122,7 @@
         <v>46055.972361111111</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>774</v>
       </c>
@@ -23213,7 +23220,7 @@
         <v>46058.87777777778</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1021</v>
       </c>
@@ -23311,7 +23318,7 @@
         <v>46058.878472222219</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>280</v>
       </c>
@@ -23409,7 +23416,7 @@
         <v>46070.497916666667</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>2844</v>
       </c>
@@ -23480,7 +23487,7 @@
         <v>46055.719513888886</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2841</v>
       </c>
@@ -23551,7 +23558,7 @@
         <v>46055.719513888886</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>2833</v>
       </c>
@@ -23622,7 +23629,7 @@
         <v>46055.660671296297</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>2829</v>
       </c>
@@ -23690,7 +23697,7 @@
         <v>46055.466215277775</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>2825</v>
       </c>
@@ -23758,7 +23765,7 @@
         <v>46055.466215277775</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1001</v>
       </c>
@@ -23856,7 +23863,7 @@
         <v>46064.372916666667</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>702</v>
       </c>
@@ -23954,7 +23961,7 @@
         <v>46066.511805555558</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>2811</v>
       </c>
@@ -24031,7 +24038,7 @@
         <v>46054.985833333332</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2807</v>
       </c>
@@ -24108,7 +24115,7 @@
         <v>46054.985833333332</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>2800</v>
       </c>
@@ -24330,7 +24337,7 @@
         <v>46054.793182870373</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>2781</v>
       </c>
@@ -24404,7 +24411,7 @@
         <v>46054.685671296298</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -24502,7 +24509,7 @@
         <v>46058.843055555553</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>879</v>
       </c>
@@ -24600,7 +24607,7 @@
         <v>46059.932638888888</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>2770</v>
       </c>
@@ -24674,7 +24681,7 @@
         <v>46054.660868055558</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1061</v>
       </c>
@@ -24766,7 +24773,7 @@
         <v>46060.349305555559</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1063</v>
       </c>
@@ -24858,7 +24865,7 @@
         <v>46068.944444444445</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>874</v>
       </c>
@@ -24953,7 +24960,7 @@
         <v>46058.882638888892</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>97</v>
       </c>
@@ -25048,7 +25055,7 @@
         <v>46058.800694444442</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>694</v>
       </c>
@@ -25143,7 +25150,7 @@
         <v>46067.670138888891</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>689</v>
       </c>
@@ -25238,7 +25245,7 @@
         <v>46067.670138888891</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1038</v>
       </c>
@@ -25339,7 +25346,7 @@
         <v>46062.859722222223</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1043</v>
       </c>
@@ -25437,7 +25444,7 @@
         <v>46062.859722222223</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -25535,7 +25542,7 @@
         <v>46067.321527777778</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -25633,7 +25640,7 @@
         <v>46058.814583333333</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>2726</v>
       </c>
@@ -25704,7 +25711,7 @@
         <v>46053.790567129632</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>545</v>
       </c>
@@ -25799,7 +25806,7 @@
         <v>46063.711111111108</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>2719</v>
       </c>
@@ -25873,7 +25880,7 @@
         <v>46053.692071759258</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1554</v>
       </c>
@@ -25947,7 +25954,7 @@
         <v>46053.692071759258</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>907</v>
       </c>
@@ -26039,7 +26046,7 @@
         <v>46070.395833333336</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -26131,7 +26138,7 @@
         <v>46058.841666666667</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>2710</v>
       </c>
@@ -26211,7 +26218,7 @@
         <v>46053.620208333334</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>2707</v>
       </c>
@@ -26291,7 +26298,7 @@
         <v>46053.620208333334</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>794</v>
       </c>
@@ -26392,7 +26399,7 @@
         <v>46055.765972222223</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>641</v>
       </c>
@@ -26487,7 +26494,7 @@
         <v>46058.863194444442</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>290</v>
       </c>
@@ -26585,7 +26592,7 @@
         <v>46070.415277777778</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>285</v>
       </c>
@@ -26683,7 +26690,7 @@
         <v>46070.412499999999</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>991</v>
       </c>
@@ -26784,7 +26791,7 @@
         <v>46055.45208333333</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>2683</v>
       </c>
@@ -26861,7 +26868,7 @@
         <v>46052.584432870368</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1966</v>
       </c>
@@ -26938,7 +26945,7 @@
         <v>46052.452928240738</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>189</v>
       </c>
@@ -27036,7 +27043,7 @@
         <v>46067.854861111111</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>2673</v>
       </c>
@@ -27107,7 +27114,7 @@
         <v>46051.801585648151</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>2667</v>
       </c>
@@ -27178,7 +27185,7 @@
         <v>46051.795648148145</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>343</v>
       </c>
@@ -27273,7 +27280,7 @@
         <v>46059.491666666669</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>2660</v>
       </c>
@@ -27347,7 +27354,7 @@
         <v>46051.572268518517</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>2658</v>
       </c>
@@ -27418,7 +27425,7 @@
         <v>46051.572268518517</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>2650</v>
       </c>
@@ -27492,7 +27499,7 @@
         <v>46051.385370370372</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>315</v>
       </c>
@@ -27590,7 +27597,7 @@
         <v>46063.38958333333</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>320</v>
       </c>
@@ -27688,7 +27695,7 @@
         <v>46063.38958333333</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1050</v>
       </c>
@@ -27783,7 +27790,7 @@
         <v>46070.625</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>836</v>
       </c>
@@ -27878,7 +27885,7 @@
         <v>46070.643750000003</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>986</v>
       </c>
@@ -27970,7 +27977,7 @@
         <v>46062.874305555553</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2628</v>
       </c>
@@ -28038,7 +28045,7 @@
         <v>46050.86791666667</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>270</v>
       </c>
@@ -28139,7 +28146,7 @@
         <v>46063.754166666666</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>2619</v>
       </c>
@@ -28216,7 +28223,7 @@
         <v>46050.849895833337</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>2612</v>
       </c>
@@ -28284,7 +28291,7 @@
         <v>46050.807673611111</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>2608</v>
       </c>
@@ -28352,7 +28359,7 @@
         <v>46050.807673611111</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>1033</v>
       </c>
@@ -28447,7 +28454,7 @@
         <v>46058.782638888886</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>809</v>
       </c>
@@ -28542,7 +28549,7 @@
         <v>46058.84097222222</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>473</v>
       </c>
@@ -28637,7 +28644,7 @@
         <v>46058.852777777778</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>941</v>
       </c>
@@ -28732,7 +28739,7 @@
         <v>46058.799305555556</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>2586</v>
       </c>
@@ -28806,7 +28813,7 @@
         <v>46049.741342592592</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>2584</v>
       </c>
@@ -28880,7 +28887,7 @@
         <v>46049.741342592592</v>
       </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>2575</v>
       </c>
@@ -28951,7 +28958,7 @@
         <v>46049.302476851852</v>
       </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>2572</v>
       </c>
@@ -29022,7 +29029,7 @@
         <v>46049.302476851852</v>
       </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>965</v>
       </c>
@@ -29117,7 +29124,7 @@
         <v>46048.754861111112</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>970</v>
       </c>
@@ -29212,7 +29219,7 @@
         <v>46048.754861111112</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>2556</v>
       </c>
@@ -29286,7 +29293,7 @@
         <v>46048.650659722225</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>2554</v>
       </c>
@@ -29360,7 +29367,7 @@
         <v>46048.650659722225</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>853</v>
       </c>
@@ -29458,7 +29465,7 @@
         <v>46048.521527777775</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>912</v>
       </c>
@@ -29556,7 +29563,7 @@
         <v>46070.395833333336</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>2539</v>
       </c>
@@ -29630,7 +29637,7 @@
         <v>46046.720833333333</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>463</v>
       </c>
@@ -29728,7 +29735,7 @@
         <v>46069.018750000003</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>2531</v>
       </c>
@@ -29802,7 +29809,7 @@
         <v>46044.918437499997</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>2522</v>
       </c>
@@ -29876,7 +29883,7 @@
         <v>46044.907835648148</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>2519</v>
       </c>
@@ -29950,7 +29957,7 @@
         <v>46044.907835648148</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>2511</v>
       </c>
@@ -30024,7 +30031,7 @@
         <v>46044.533807870372</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>396</v>
       </c>
@@ -30119,7 +30126,7 @@
         <v>46058.862500000003</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>391</v>
       </c>
@@ -30217,7 +30224,7 @@
         <v>46058.862500000003</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>757</v>
       </c>
@@ -30309,7 +30316,7 @@
         <v>46060.384027777778</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>761</v>
       </c>
@@ -30398,7 +30405,7 @@
         <v>46060.384027777778</v>
       </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>432</v>
       </c>
@@ -30499,7 +30506,7 @@
         <v>46070.311111111114</v>
       </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>437</v>
       </c>
@@ -30600,7 +30607,7 @@
         <v>46070.311111111114</v>
       </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>2487</v>
       </c>
@@ -30677,7 +30684,7 @@
         <v>46043.679756944446</v>
       </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>19</v>
       </c>
@@ -30778,7 +30785,7 @@
         <v>46058.798611111109</v>
       </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>2480</v>
       </c>
@@ -30849,7 +30856,7 @@
         <v>46043.604131944441</v>
       </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>2477</v>
       </c>
@@ -30920,7 +30927,7 @@
         <v>46043.604131944441</v>
       </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>868</v>
       </c>
@@ -31018,7 +31025,7 @@
         <v>46067.814583333333</v>
       </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>2469</v>
       </c>
@@ -31092,7 +31099,7 @@
         <v>46043.600601851853</v>
       </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>736</v>
       </c>
@@ -31184,7 +31191,7 @@
         <v>46061.644444444442</v>
       </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>731</v>
       </c>
@@ -31276,7 +31283,7 @@
         <v>46061.738194444442</v>
       </c>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>2455</v>
       </c>
@@ -31350,7 +31357,7 @@
         <v>46042.323275462964</v>
       </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>2453</v>
       </c>
@@ -31424,7 +31431,7 @@
         <v>46042.323275462964</v>
       </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>142</v>
       </c>
@@ -31522,7 +31529,7 @@
         <v>46059.150694444441</v>
       </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>2444</v>
       </c>
@@ -31596,7 +31603,7 @@
         <v>46041.795682870368</v>
       </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>542</v>
       </c>
@@ -31691,7 +31698,7 @@
         <v>46058.859027777777</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>784</v>
       </c>
@@ -31789,7 +31796,7 @@
         <v>46058.886111111111</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>2426</v>
       </c>
@@ -31860,7 +31867,7 @@
         <v>46039.128101851849</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>848</v>
       </c>
@@ -31955,7 +31962,7 @@
         <v>46070.782638888886</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>1077</v>
       </c>
@@ -32053,7 +32060,7 @@
         <v>46058.857638888891</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>2417</v>
       </c>
@@ -32127,7 +32134,7 @@
         <v>46038.878935185188</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>537</v>
       </c>
@@ -32219,7 +32226,7 @@
         <v>46048.272222222222</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>2405</v>
       </c>
@@ -32293,7 +32300,7 @@
         <v>46038.726099537038</v>
       </c>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>60</v>
       </c>
@@ -32388,7 +32395,7 @@
         <v>46048.671527777777</v>
       </c>
     </row>
-    <row r="161" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>1059</v>
       </c>
@@ -32477,7 +32484,7 @@
         <v>46048.671527777777</v>
       </c>
     </row>
-    <row r="162" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>275</v>
       </c>
@@ -32575,7 +32582,7 @@
         <v>46058.843055555553</v>
       </c>
     </row>
-    <row r="163" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>883</v>
       </c>
@@ -32673,7 +32680,7 @@
         <v>46058.849305555559</v>
       </c>
     </row>
-    <row r="164" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>503</v>
       </c>
@@ -32771,7 +32778,7 @@
         <v>46048.669444444444</v>
       </c>
     </row>
-    <row r="165" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>1067</v>
       </c>
@@ -32863,7 +32870,7 @@
         <v>46048.669444444444</v>
       </c>
     </row>
-    <row r="166" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>660</v>
       </c>
@@ -32964,7 +32971,7 @@
         <v>46058.819444444445</v>
       </c>
     </row>
-    <row r="167" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>2371</v>
       </c>
@@ -33041,7 +33048,7 @@
         <v>46037.977488425924</v>
       </c>
     </row>
-    <row r="168" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>2362</v>
       </c>
@@ -33115,7 +33122,7 @@
         <v>46037.949270833335</v>
       </c>
     </row>
-    <row r="169" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>2360</v>
       </c>
@@ -33189,7 +33196,7 @@
         <v>46037.949270833335</v>
       </c>
     </row>
-    <row r="170" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>718</v>
       </c>
@@ -33287,7 +33294,7 @@
         <v>46056.35833333333</v>
       </c>
     </row>
-    <row r="171" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>1006</v>
       </c>
@@ -33385,7 +33392,7 @@
         <v>46063.657638888886</v>
       </c>
     </row>
-    <row r="172" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>588</v>
       </c>
@@ -33480,7 +33487,7 @@
         <v>46064.092361111114</v>
       </c>
     </row>
-    <row r="173" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>2341</v>
       </c>
@@ -33551,7 +33558,7 @@
         <v>46037.458124999997</v>
       </c>
     </row>
-    <row r="174" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>623</v>
       </c>
@@ -33646,7 +33653,7 @@
         <v>46059.177083333336</v>
       </c>
     </row>
-    <row r="175" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>446</v>
       </c>
@@ -33741,7 +33748,7 @@
         <v>46048.446527777778</v>
       </c>
     </row>
-    <row r="176" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>451</v>
       </c>
@@ -33833,7 +33840,7 @@
         <v>46048.446527777778</v>
       </c>
     </row>
-    <row r="177" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>2322</v>
       </c>
@@ -33907,7 +33914,7 @@
         <v>46037.176296296297</v>
       </c>
     </row>
-    <row r="178" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>55</v>
       </c>
@@ -34005,7 +34012,7 @@
         <v>46070.376388888886</v>
       </c>
     </row>
-    <row r="179" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>863</v>
       </c>
@@ -34103,7 +34110,7 @@
         <v>46070.376388888886</v>
       </c>
     </row>
-    <row r="180" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>2309</v>
       </c>
@@ -34177,7 +34184,7 @@
         <v>46035.790636574071</v>
       </c>
     </row>
-    <row r="181" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>2305</v>
       </c>
@@ -34251,7 +34258,7 @@
         <v>46035.790636574071</v>
       </c>
     </row>
-    <row r="182" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>827</v>
       </c>
@@ -34349,7 +34356,7 @@
         <v>46058.797222222223</v>
       </c>
     </row>
-    <row r="183" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>832</v>
       </c>
@@ -34447,7 +34454,7 @@
         <v>46058.794444444444</v>
       </c>
     </row>
-    <row r="184" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>2294</v>
       </c>
@@ -34518,7 +34525,7 @@
         <v>46035.689375000002</v>
       </c>
     </row>
-    <row r="185" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>726</v>
       </c>
@@ -34613,7 +34620,7 @@
         <v>46058.798611111109</v>
       </c>
     </row>
-    <row r="186" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>2286</v>
       </c>
@@ -34666,7 +34673,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="187" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>2283</v>
       </c>
@@ -34719,7 +34726,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="188" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>2281</v>
       </c>
@@ -34772,7 +34779,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="189" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>2278</v>
       </c>
@@ -34825,7 +34832,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="190" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>2276</v>
       </c>
@@ -34878,7 +34885,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="191" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>2274</v>
       </c>
@@ -34931,7 +34938,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="192" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>2272</v>
       </c>
@@ -34984,7 +34991,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="193" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>2268</v>
       </c>
@@ -35037,7 +35044,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="194" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>584</v>
       </c>
@@ -35114,7 +35121,7 @@
         <v>46058.881249999999</v>
       </c>
     </row>
-    <row r="195" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>579</v>
       </c>
@@ -35191,7 +35198,7 @@
         <v>46058.881249999999</v>
       </c>
     </row>
-    <row r="196" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>2258</v>
       </c>
@@ -35262,7 +35269,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="197" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>2255</v>
       </c>
@@ -35333,7 +35340,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="198" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>697</v>
       </c>
@@ -35428,7 +35435,7 @@
         <v>46064.540972222225</v>
       </c>
     </row>
-    <row r="199" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>2251</v>
       </c>
@@ -35499,7 +35506,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="200" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>952</v>
       </c>
@@ -35600,7 +35607,7 @@
         <v>46067.382638888892</v>
       </c>
     </row>
-    <row r="201" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>520</v>
       </c>
@@ -35698,7 +35705,7 @@
         <v>46067.381944444445</v>
       </c>
     </row>
-    <row r="202" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>413</v>
       </c>
@@ -35793,7 +35800,7 @@
         <v>46067.027083333334</v>
       </c>
     </row>
-    <row r="203" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>418</v>
       </c>
@@ -35888,7 +35895,7 @@
         <v>46067.027083333334</v>
       </c>
     </row>
-    <row r="204" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>494</v>
       </c>
@@ -35986,7 +35993,7 @@
         <v>46058.913194444445</v>
       </c>
     </row>
-    <row r="205" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>499</v>
       </c>
@@ -36084,7 +36091,7 @@
         <v>46058.911111111112</v>
       </c>
     </row>
-    <row r="206" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>2226</v>
       </c>
@@ -36149,7 +36156,7 @@
         <v>46033.396817129629</v>
       </c>
     </row>
-    <row r="207" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>996</v>
       </c>
@@ -36247,7 +36254,7 @@
         <v>46055.448611111111</v>
       </c>
     </row>
-    <row r="208" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>2220</v>
       </c>
@@ -36321,7 +36328,7 @@
         <v>46032.664780092593</v>
       </c>
     </row>
-    <row r="209" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>1082</v>
       </c>
@@ -36410,7 +36417,7 @@
         <v>46058.827777777777</v>
       </c>
     </row>
-    <row r="210" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>1087</v>
       </c>
@@ -36502,7 +36509,7 @@
         <v>46058.826388888891</v>
       </c>
     </row>
-    <row r="211" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>750</v>
       </c>
@@ -36597,7 +36604,7 @@
         <v>46059.338194444441</v>
       </c>
     </row>
-    <row r="212" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>746</v>
       </c>
@@ -36695,7 +36702,7 @@
         <v>46059.338194444441</v>
       </c>
     </row>
-    <row r="213" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>52</v>
       </c>
@@ -36793,7 +36800,7 @@
         <v>46063.984027777777</v>
       </c>
     </row>
-    <row r="214" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>48</v>
       </c>
@@ -36891,7 +36898,7 @@
         <v>46063.984027777777</v>
       </c>
     </row>
-    <row r="215" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>655</v>
       </c>
@@ -36989,7 +36996,7 @@
         <v>46060.875694444447</v>
       </c>
     </row>
-    <row r="216" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>1069</v>
       </c>
@@ -37081,7 +37088,7 @@
         <v>46060.875694444447</v>
       </c>
     </row>
-    <row r="217" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>2184</v>
       </c>
@@ -37158,7 +37165,7 @@
         <v>46030.965729166666</v>
       </c>
     </row>
-    <row r="218" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -37259,7 +37266,7 @@
         <v>46061.171527777777</v>
       </c>
     </row>
-    <row r="219" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>779</v>
       </c>
@@ -37354,7 +37361,7 @@
         <v>46049.840277777781</v>
       </c>
     </row>
-    <row r="220" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>1025</v>
       </c>
@@ -37449,7 +37456,7 @@
         <v>46060.259722222225</v>
       </c>
     </row>
-    <row r="221" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>2168</v>
       </c>
@@ -37523,7 +37530,7 @@
         <v>46030.596400462964</v>
       </c>
     </row>
-    <row r="222" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>2160</v>
       </c>
@@ -37597,7 +37604,7 @@
         <v>46030.385347222225</v>
       </c>
     </row>
-    <row r="223" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>2158</v>
       </c>
@@ -37674,7 +37681,7 @@
         <v>46030.385347222225</v>
       </c>
     </row>
-    <row r="224" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>2149</v>
       </c>
@@ -37748,7 +37755,7 @@
         <v>46030.35796296296</v>
       </c>
     </row>
-    <row r="225" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>179</v>
       </c>
@@ -37846,7 +37853,7 @@
         <v>46048.746527777781</v>
       </c>
     </row>
-    <row r="226" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>73</v>
       </c>
@@ -37941,7 +37948,7 @@
         <v>46067.788194444445</v>
       </c>
     </row>
-    <row r="227" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>78</v>
       </c>
@@ -38036,7 +38043,7 @@
         <v>46069.304861111108</v>
       </c>
     </row>
-    <row r="228" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>478</v>
       </c>
@@ -38131,7 +38138,7 @@
         <v>46063.263888888891</v>
       </c>
     </row>
-    <row r="229" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>483</v>
       </c>
@@ -38223,7 +38230,7 @@
         <v>46063.263888888891</v>
       </c>
     </row>
-    <row r="230" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>2128</v>
       </c>
@@ -38297,7 +38304,7 @@
         <v>46029.817777777775</v>
       </c>
     </row>
-    <row r="231" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>2125</v>
       </c>
@@ -38371,7 +38378,7 @@
         <v>46029.817777777775</v>
       </c>
     </row>
-    <row r="232" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>213</v>
       </c>
@@ -38466,7 +38473,7 @@
         <v>46066.103472222225</v>
       </c>
     </row>
-    <row r="233" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>65</v>
       </c>
@@ -38564,7 +38571,7 @@
         <v>46051.777083333334</v>
       </c>
     </row>
-    <row r="234" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>70</v>
       </c>
@@ -38659,7 +38666,7 @@
         <v>46051.777083333334</v>
       </c>
     </row>
-    <row r="235" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>2103</v>
       </c>
@@ -38736,7 +38743,7 @@
         <v>46029.32534722222</v>
       </c>
     </row>
-    <row r="236" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>2102</v>
       </c>
@@ -38813,7 +38820,7 @@
         <v>46029.32534722222</v>
       </c>
     </row>
-    <row r="237" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>822</v>
       </c>
@@ -38911,7 +38918,7 @@
         <v>46068.82916666667</v>
       </c>
     </row>
-    <row r="238" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>121</v>
       </c>
@@ -39012,7 +39019,7 @@
         <v>46060.910416666666</v>
       </c>
     </row>
-    <row r="239" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>116</v>
       </c>
@@ -39113,7 +39120,7 @@
         <v>46058.79791666667</v>
       </c>
     </row>
-    <row r="240" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>2081</v>
       </c>
@@ -39190,7 +39197,7 @@
         <v>46028.743807870371</v>
       </c>
     </row>
-    <row r="241" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>564</v>
       </c>
@@ -39291,7 +39298,7 @@
         <v>46059.578472222223</v>
       </c>
     </row>
-    <row r="242" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>770</v>
       </c>
@@ -39386,7 +39393,7 @@
         <v>46059.174305555556</v>
       </c>
     </row>
-    <row r="243" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>752</v>
       </c>
@@ -39481,7 +39488,7 @@
         <v>46058.88958333333</v>
       </c>
     </row>
-    <row r="244" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>184</v>
       </c>
@@ -39576,7 +39583,7 @@
         <v>46062.370833333334</v>
       </c>
     </row>
-    <row r="245" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>932</v>
       </c>
@@ -39671,7 +39678,7 @@
         <v>46059.512499999997</v>
       </c>
     </row>
-    <row r="246" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>1071</v>
       </c>
@@ -39763,7 +39770,7 @@
         <v>46059.512499999997</v>
       </c>
     </row>
-    <row r="247" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>922</v>
       </c>
@@ -39861,7 +39868,7 @@
         <v>46064.795138888891</v>
       </c>
     </row>
-    <row r="248" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>408</v>
       </c>
@@ -39959,7 +39966,7 @@
         <v>46064.792361111111</v>
       </c>
     </row>
-    <row r="249" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>2048</v>
       </c>
@@ -40033,7 +40040,7 @@
         <v>46027.813958333332</v>
       </c>
     </row>
-    <row r="250" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>2046</v>
       </c>
@@ -40107,7 +40114,7 @@
         <v>46027.813958333332</v>
       </c>
     </row>
-    <row r="251" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>2038</v>
       </c>
@@ -40178,7 +40185,7 @@
         <v>46027.802372685182</v>
       </c>
     </row>
-    <row r="252" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>2034</v>
       </c>
@@ -40249,7 +40256,7 @@
         <v>46027.802372685182</v>
       </c>
     </row>
-    <row r="253" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>2027</v>
       </c>
@@ -40320,7 +40327,7 @@
         <v>46027.547835648147</v>
       </c>
     </row>
-    <row r="254" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>2025</v>
       </c>
@@ -40391,7 +40398,7 @@
         <v>46027.547835648147</v>
       </c>
     </row>
-    <row r="255" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>2017</v>
       </c>
@@ -40459,7 +40466,7 @@
         <v>46027.363252314812</v>
       </c>
     </row>
-    <row r="256" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>137</v>
       </c>
@@ -40551,7 +40558,7 @@
         <v>46061.425694444442</v>
       </c>
     </row>
-    <row r="257" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>33</v>
       </c>
@@ -40646,7 +40653,7 @@
         <v>46062.732638888891</v>
       </c>
     </row>
-    <row r="258" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>38</v>
       </c>
@@ -40744,7 +40751,7 @@
         <v>46062.763888888891</v>
       </c>
     </row>
-    <row r="259" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>170</v>
       </c>
@@ -40839,7 +40846,7 @@
         <v>46068.6875</v>
       </c>
     </row>
-    <row r="260" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>165</v>
       </c>
@@ -40934,7 +40941,7 @@
         <v>46058.84652777778</v>
       </c>
     </row>
-    <row r="261" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>369</v>
       </c>
@@ -41029,7 +41036,7 @@
         <v>46048.377083333333</v>
       </c>
     </row>
-    <row r="262" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>1989</v>
       </c>
@@ -41106,7 +41113,7 @@
         <v>46026.667337962965</v>
       </c>
     </row>
-    <row r="263" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>1986</v>
       </c>
@@ -41183,7 +41190,7 @@
         <v>46026.667337962965</v>
       </c>
     </row>
-    <row r="264" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>1977</v>
       </c>
@@ -41254,7 +41261,7 @@
         <v>46026.546076388891</v>
       </c>
     </row>
-    <row r="265" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>1974</v>
       </c>
@@ -41325,7 +41332,7 @@
         <v>46026.546076388891</v>
       </c>
     </row>
-    <row r="266" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>1966</v>
       </c>
@@ -41399,7 +41406,7 @@
         <v>46026.415127314816</v>
       </c>
     </row>
-    <row r="267" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>1958</v>
       </c>
@@ -41476,7 +41483,7 @@
         <v>46025.551689814813</v>
       </c>
     </row>
-    <row r="268" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>1956</v>
       </c>
@@ -41553,7 +41560,7 @@
         <v>46025.551689814813</v>
       </c>
     </row>
-    <row r="269" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>1946</v>
       </c>
@@ -41627,7 +41634,7 @@
         <v>46025.475324074076</v>
       </c>
     </row>
-    <row r="270" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>684</v>
       </c>
@@ -41725,7 +41732,7 @@
         <v>46058.804166666669</v>
       </c>
     </row>
-    <row r="271" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>1938</v>
       </c>
@@ -41799,7 +41806,7 @@
         <v>46025.337488425925</v>
       </c>
     </row>
-    <row r="272" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>242</v>
       </c>
@@ -41891,7 +41898,7 @@
         <v>46049.095833333333</v>
       </c>
     </row>
-    <row r="273" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>763</v>
       </c>
@@ -41989,7 +41996,7 @@
         <v>46069.995833333334</v>
       </c>
     </row>
-    <row r="274" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>1925</v>
       </c>
@@ -42063,7 +42070,7 @@
         <v>46024.680902777778</v>
       </c>
     </row>
-    <row r="275" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>960</v>
       </c>
@@ -42161,7 +42168,7 @@
         <v>46058.86041666667</v>
       </c>
     </row>
-    <row r="276" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>1916</v>
       </c>
@@ -42235,7 +42242,7 @@
         <v>46024.661793981482</v>
       </c>
     </row>
-    <row r="277" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>1045</v>
       </c>
@@ -42333,7 +42340,7 @@
         <v>46054.898611111108</v>
       </c>
     </row>
-    <row r="278" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>818</v>
       </c>
@@ -42431,7 +42438,7 @@
         <v>46058.834722222222</v>
       </c>
     </row>
-    <row r="279" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>1899</v>
       </c>
@@ -42502,7 +42509,7 @@
         <v>46024.514236111114</v>
       </c>
     </row>
-    <row r="280" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>1897</v>
       </c>
@@ -42573,7 +42580,7 @@
         <v>46024.514236111114</v>
       </c>
     </row>
-    <row r="281" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>1888</v>
       </c>
@@ -42647,7 +42654,7 @@
         <v>46024.512673611112</v>
       </c>
     </row>
-    <row r="282" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>1885</v>
       </c>
@@ -42721,7 +42728,7 @@
         <v>46024.512673611112</v>
       </c>
     </row>
-    <row r="283" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>1065</v>
       </c>
@@ -42810,7 +42817,7 @@
         <v>46049.750694444447</v>
       </c>
     </row>
-    <row r="284" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>355</v>
       </c>
@@ -42905,7 +42912,7 @@
         <v>46049.750694444447</v>
       </c>
     </row>
-    <row r="285" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>1870</v>
       </c>
@@ -42976,7 +42983,7 @@
         <v>46023.938506944447</v>
       </c>
     </row>
-    <row r="286" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>1868</v>
       </c>
@@ -43047,7 +43054,7 @@
         <v>46023.938506944447</v>
       </c>
     </row>
-    <row r="287" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>1862</v>
       </c>
@@ -43118,7 +43125,7 @@
         <v>46023.802141203705</v>
       </c>
     </row>
-    <row r="288" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>1859</v>
       </c>
@@ -43189,7 +43196,7 @@
         <v>46023.802141203705</v>
       </c>
     </row>
-    <row r="289" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>194</v>
       </c>
@@ -43287,7 +43294,7 @@
         <v>46065.164583333331</v>
       </c>
     </row>
-    <row r="290" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>1850</v>
       </c>
@@ -43361,7 +43368,7 @@
         <v>46023.711574074077</v>
       </c>
     </row>
-    <row r="291" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>1842</v>
       </c>
@@ -43435,7 +43442,7 @@
         <v>46023.609699074077</v>
       </c>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>559</v>
       </c>
@@ -43530,7 +43537,7 @@
         <v>46062.680555555555</v>
       </c>
     </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>1833</v>
       </c>
@@ -43601,7 +43608,7 @@
         <v>46023.586215277777</v>
       </c>
     </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>621</v>
       </c>
@@ -43696,7 +43703,7 @@
         <v>46048.813888888886</v>
       </c>
     </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>616</v>
       </c>
@@ -43794,7 +43801,7 @@
         <v>46048.813888888886</v>
       </c>
     </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>199</v>
       </c>
@@ -43895,7 +43902,7 @@
         <v>46060.936111111114</v>
       </c>
     </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>1817</v>
       </c>
@@ -43972,7 +43979,7 @@
         <v>46023.50953703704</v>
       </c>
     </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>593</v>
       </c>
@@ -44064,7 +44071,7 @@
         <v>46067.547222222223</v>
       </c>
     </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>265</v>
       </c>
@@ -44165,7 +44172,7 @@
         <v>46068.813888888886</v>
       </c>
     </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>902</v>
       </c>
@@ -44260,7 +44267,7 @@
         <v>46051.645138888889</v>
       </c>
     </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>1791</v>
       </c>
@@ -44331,7 +44338,7 @@
         <v>46023.475659722222</v>
       </c>
     </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>209</v>
       </c>
@@ -44423,7 +44430,7 @@
         <v>46067.356249999997</v>
       </c>
     </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>204</v>
       </c>
@@ -44515,7 +44522,7 @@
         <v>46067.356249999997</v>
       </c>
     </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>1777</v>
       </c>
@@ -44589,7 +44596,7 @@
         <v>46022.338703703703</v>
       </c>
     </row>
-    <row r="305" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>1776</v>
       </c>
@@ -44663,7 +44670,7 @@
         <v>46022.338703703703</v>
       </c>
     </row>
-    <row r="306" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>158</v>
       </c>
@@ -44758,7 +44765,7 @@
         <v>46048.445833333331</v>
       </c>
     </row>
-    <row r="307" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>163</v>
       </c>
@@ -44850,7 +44857,7 @@
         <v>46048.445833333331</v>
       </c>
     </row>
-    <row r="308" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>976</v>
       </c>
@@ -44948,7 +44955,7 @@
         <v>46059.542361111111</v>
       </c>
     </row>
-    <row r="309" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>574</v>
       </c>
@@ -45046,7 +45053,7 @@
         <v>46059.974305555559</v>
       </c>
     </row>
-    <row r="310" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>147</v>
       </c>
@@ -45138,7 +45145,7 @@
         <v>46059.463888888888</v>
       </c>
     </row>
-    <row r="311" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>152</v>
       </c>
@@ -45227,7 +45234,7 @@
         <v>46059.463888888888</v>
       </c>
     </row>
-    <row r="312" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>1748</v>
       </c>
@@ -45298,7 +45305,7 @@
         <v>46021.842534722222</v>
       </c>
     </row>
-    <row r="313" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>1745</v>
       </c>
@@ -45369,7 +45376,7 @@
         <v>46021.842534722222</v>
       </c>
     </row>
-    <row r="314" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>92</v>
       </c>
@@ -45470,7 +45477,7 @@
         <v>46061.823611111111</v>
       </c>
     </row>
-    <row r="315" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>1734</v>
       </c>
@@ -45544,7 +45551,7 @@
         <v>46021.838252314818</v>
       </c>
     </row>
-    <row r="316" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>1726</v>
       </c>
@@ -45618,7 +45625,7 @@
         <v>46020.877951388888</v>
       </c>
     </row>
-    <row r="317" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>1723</v>
       </c>
@@ -45692,7 +45699,7 @@
         <v>46020.877951388888</v>
       </c>
     </row>
-    <row r="318" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>633</v>
       </c>
@@ -45787,7 +45794,7 @@
         <v>46064.495138888888</v>
       </c>
     </row>
-    <row r="319" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>638</v>
       </c>
@@ -45882,7 +45889,7 @@
         <v>46064.495138888888</v>
       </c>
     </row>
-    <row r="320" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>1709</v>
       </c>
@@ -45956,7 +45963,7 @@
         <v>46020.45820601852</v>
       </c>
     </row>
-    <row r="321" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>843</v>
       </c>
@@ -46054,7 +46061,7 @@
         <v>46048.336111111108</v>
       </c>
     </row>
-    <row r="322" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>1701</v>
       </c>
@@ -46128,7 +46135,7 @@
         <v>46019.362071759257</v>
       </c>
     </row>
-    <row r="323" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>893</v>
       </c>
@@ -46226,7 +46233,7 @@
         <v>46067.751388888886</v>
       </c>
     </row>
-    <row r="324" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>1695</v>
       </c>
@@ -46300,7 +46307,7 @@
         <v>46019.283310185187</v>
       </c>
     </row>
-    <row r="325" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>1688</v>
       </c>
@@ -46371,7 +46378,7 @@
         <v>46018.70453703704</v>
       </c>
     </row>
-    <row r="326" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>706</v>
       </c>
@@ -46469,7 +46476,7 @@
         <v>46060.53125</v>
       </c>
     </row>
-    <row r="327" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>711</v>
       </c>
@@ -46564,7 +46571,7 @@
         <v>46060.53125</v>
       </c>
     </row>
-    <row r="328" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>1674</v>
       </c>
@@ -46635,7 +46642,7 @@
         <v>46017.395543981482</v>
       </c>
     </row>
-    <row r="329" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>766</v>
       </c>
@@ -46730,7 +46737,7 @@
         <v>46062.729166666664</v>
       </c>
     </row>
-    <row r="330" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>398</v>
       </c>
@@ -46828,7 +46835,7 @@
         <v>46061.180555555555</v>
       </c>
     </row>
-    <row r="331" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>915</v>
       </c>
@@ -46926,7 +46933,7 @@
         <v>46048.520138888889</v>
       </c>
     </row>
-    <row r="332" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>1659</v>
       </c>
@@ -46997,7 +47004,7 @@
         <v>46017.269490740742</v>
       </c>
     </row>
-    <row r="333" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>1655</v>
       </c>
@@ -47068,7 +47075,7 @@
         <v>46017.269490740742</v>
       </c>
     </row>
-    <row r="334" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>740</v>
       </c>
@@ -47163,7 +47170,7 @@
         <v>46048.59375</v>
       </c>
     </row>
-    <row r="335" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>744</v>
       </c>
@@ -47255,7 +47262,7 @@
         <v>46048.59375</v>
       </c>
     </row>
-    <row r="336" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>1641</v>
       </c>
@@ -47326,7 +47333,7 @@
         <v>46015.84302083333</v>
       </c>
     </row>
-    <row r="337" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>1638</v>
       </c>
@@ -47397,7 +47404,7 @@
         <v>46015.84302083333</v>
       </c>
     </row>
-    <row r="338" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>218</v>
       </c>
@@ -47495,7 +47502,7 @@
         <v>46063.810416666667</v>
       </c>
     </row>
-    <row r="339" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>1629</v>
       </c>
@@ -47572,7 +47579,7 @@
         <v>46015.784236111111</v>
       </c>
     </row>
-    <row r="340" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>1029</v>
       </c>
@@ -47670,7 +47677,7 @@
         <v>46069.706250000003</v>
       </c>
     </row>
-    <row r="341" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>789</v>
       </c>
@@ -47768,7 +47775,7 @@
         <v>46069.700694444444</v>
       </c>
     </row>
-    <row r="342" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>1613</v>
       </c>
@@ -47842,7 +47849,7 @@
         <v>46015.679305555554</v>
       </c>
     </row>
-    <row r="343" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>441</v>
       </c>
@@ -47940,7 +47947,7 @@
         <v>46064.816666666666</v>
       </c>
     </row>
-    <row r="344" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>1074</v>
       </c>
@@ -48038,7 +48045,7 @@
         <v>46049.790277777778</v>
       </c>
     </row>
-    <row r="345" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>421</v>
       </c>
@@ -48133,7 +48140,7 @@
         <v>46049.790277777778</v>
       </c>
     </row>
-    <row r="346" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>425</v>
       </c>
@@ -48231,7 +48238,7 @@
         <v>46048.401388888888</v>
       </c>
     </row>
-    <row r="347" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>430</v>
       </c>
@@ -48326,7 +48333,7 @@
         <v>46048.401388888888</v>
       </c>
     </row>
-    <row r="348" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>1590</v>
       </c>
@@ -48400,7 +48407,7 @@
         <v>46015.439131944448</v>
       </c>
     </row>
-    <row r="349" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>1587</v>
       </c>
@@ -48474,7 +48481,7 @@
         <v>46015.439131944448</v>
       </c>
     </row>
-    <row r="350" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>1579</v>
       </c>
@@ -48548,7 +48555,7 @@
         <v>46015.433900462966</v>
       </c>
     </row>
-    <row r="351" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>1576</v>
       </c>
@@ -48622,7 +48629,7 @@
         <v>46015.433900462966</v>
       </c>
     </row>
-    <row r="352" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>1568</v>
       </c>
@@ -48693,7 +48700,7 @@
         <v>46015.337905092594</v>
       </c>
     </row>
-    <row r="353" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>1565</v>
       </c>
@@ -48764,7 +48771,7 @@
         <v>46015.337905092594</v>
       </c>
     </row>
-    <row r="354" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>1556</v>
       </c>
@@ -48838,7 +48845,7 @@
         <v>46014.740243055552</v>
       </c>
     </row>
-    <row r="355" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>1554</v>
       </c>
@@ -48912,7 +48919,7 @@
         <v>46014.740243055552</v>
       </c>
     </row>
-    <row r="356" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>299</v>
       </c>
@@ -49010,7 +49017,7 @@
         <v>46070.581944444442</v>
       </c>
     </row>
-    <row r="357" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>304</v>
       </c>
@@ -49108,7 +49115,7 @@
         <v>46060.904861111114</v>
       </c>
     </row>
-    <row r="358" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>1539</v>
       </c>
@@ -49182,7 +49189,7 @@
         <v>46013.485590277778</v>
       </c>
     </row>
-    <row r="359" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>1535</v>
       </c>
@@ -49256,7 +49263,7 @@
         <v>46013.485590277778</v>
       </c>
     </row>
-    <row r="360" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>1527</v>
       </c>
@@ -49330,7 +49337,7 @@
         <v>46013.406481481485</v>
       </c>
     </row>
-    <row r="361" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>1523</v>
       </c>
@@ -49404,7 +49411,7 @@
         <v>46013.406481481485</v>
       </c>
     </row>
-    <row r="362" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>981</v>
       </c>
@@ -49499,7 +49506,7 @@
         <v>46068.129861111112</v>
       </c>
     </row>
-    <row r="363" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>1510</v>
       </c>
@@ -49570,7 +49577,7 @@
         <v>46012.645243055558</v>
       </c>
     </row>
-    <row r="364" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>669</v>
       </c>
@@ -49668,7 +49675,7 @@
         <v>46058.915277777778</v>
       </c>
     </row>
-    <row r="365" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>674</v>
       </c>
@@ -49766,7 +49773,7 @@
         <v>46058.918055555558</v>
       </c>
     </row>
-    <row r="366" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>948</v>
       </c>
@@ -49864,7 +49871,7 @@
         <v>46065.861805555556</v>
       </c>
     </row>
-    <row r="367" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>508</v>
       </c>
@@ -49962,7 +49969,7 @@
         <v>46065.852083333331</v>
       </c>
     </row>
-    <row r="368" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>1054</v>
       </c>
@@ -50060,7 +50067,7 @@
         <v>46059.650694444441</v>
       </c>
     </row>
-    <row r="369" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>858</v>
       </c>
@@ -50158,7 +50165,7 @@
         <v>46048.498611111114</v>
       </c>
     </row>
-    <row r="370" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>1483</v>
       </c>
@@ -50229,7 +50236,7 @@
         <v>46011.53396990741</v>
       </c>
     </row>
-    <row r="371" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>1479</v>
       </c>
@@ -50300,7 +50307,7 @@
         <v>46011.53396990741</v>
       </c>
     </row>
-    <row r="372" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>678</v>
       </c>
@@ -50398,7 +50405,7 @@
         <v>46063.842361111114</v>
       </c>
     </row>
-    <row r="373" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>682</v>
       </c>
@@ -50493,7 +50500,7 @@
         <v>46063.842361111114</v>
       </c>
     </row>
-    <row r="374" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>468</v>
       </c>
@@ -50588,7 +50595,7 @@
         <v>46058.819444444445</v>
       </c>
     </row>
-    <row r="375" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>1458</v>
       </c>
@@ -50662,7 +50669,7 @@
         <v>46011.46434027778</v>
       </c>
     </row>
-    <row r="376" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>1455</v>
       </c>
@@ -50736,7 +50743,7 @@
         <v>46011.46434027778</v>
       </c>
     </row>
-    <row r="377" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>1447</v>
       </c>
@@ -50810,7 +50817,7 @@
         <v>46010.715671296297</v>
       </c>
     </row>
-    <row r="378" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>814</v>
       </c>
@@ -50905,7 +50912,7 @@
         <v>46059.905555555553</v>
       </c>
     </row>
-    <row r="379" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>956</v>
       </c>
@@ -51003,7 +51010,7 @@
         <v>46058.847222222219</v>
       </c>
     </row>
-    <row r="380" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>532</v>
       </c>
@@ -51101,7 +51108,7 @@
         <v>46058.80972222222</v>
       </c>
     </row>
-    <row r="381" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>129</v>
       </c>
@@ -51199,7 +51206,7 @@
         <v>46057.831250000003</v>
       </c>
     </row>
-    <row r="382" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>134</v>
       </c>
@@ -51297,7 +51304,7 @@
         <v>46057.833333333336</v>
       </c>
     </row>
-    <row r="383" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>1418</v>
       </c>
@@ -51368,7 +51375,7 @@
         <v>46009.492037037038</v>
       </c>
     </row>
-    <row r="384" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>1415</v>
       </c>
@@ -51439,7 +51446,7 @@
         <v>46009.492037037038</v>
       </c>
     </row>
-    <row r="385" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>799</v>
       </c>
@@ -51537,7 +51544,7 @@
         <v>46048.543055555558</v>
       </c>
     </row>
-    <row r="386" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>1399</v>
       </c>
@@ -51611,7 +51618,7 @@
         <v>46008.904687499999</v>
       </c>
     </row>
-    <row r="387" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>1397</v>
       </c>
@@ -51685,7 +51692,7 @@
         <v>46008.904687499999</v>
       </c>
     </row>
-    <row r="388" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>1388</v>
       </c>
@@ -51759,7 +51766,7 @@
         <v>46008.810729166667</v>
       </c>
     </row>
-    <row r="389" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>1387</v>
       </c>
@@ -51833,7 +51840,7 @@
         <v>46008.810729166667</v>
       </c>
     </row>
-    <row r="390" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>888</v>
       </c>
@@ -51931,7 +51938,7 @@
         <v>46069.885416666664</v>
       </c>
     </row>
-    <row r="391" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>294</v>
       </c>
@@ -52029,7 +52036,7 @@
         <v>46069.888194444444</v>
       </c>
     </row>
-    <row r="392" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>607</v>
       </c>
@@ -52124,7 +52131,7 @@
         <v>46067.271527777775</v>
       </c>
     </row>
-    <row r="393" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>612</v>
       </c>
@@ -52412,7 +52419,7 @@
         <v>46059.365972222222</v>
       </c>
     </row>
-    <row r="396" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>328</v>
       </c>
@@ -52507,7 +52514,7 @@
         <v>46060.349305555559</v>
       </c>
     </row>
-    <row r="397" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>333</v>
       </c>
@@ -52602,7 +52609,7 @@
         <v>46068.944444444445</v>
       </c>
     </row>
-    <row r="398" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>374</v>
       </c>
@@ -52703,7 +52710,7 @@
         <v>46048.487500000003</v>
       </c>
     </row>
-    <row r="399" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>384</v>
       </c>
@@ -52801,7 +52808,7 @@
         <v>46059.345138888886</v>
       </c>
     </row>
-    <row r="400" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>389</v>
       </c>
@@ -52896,7 +52903,7 @@
         <v>46059.345138888886</v>
       </c>
     </row>
-    <row r="401" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>1344</v>
       </c>
@@ -52970,7 +52977,7 @@
         <v>46008.496446759258</v>
       </c>
     </row>
-    <row r="402" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>237</v>
       </c>
@@ -53071,7 +53078,7 @@
         <v>46048.377083333333</v>
       </c>
     </row>
-    <row r="403" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>1016</v>
       </c>
@@ -53169,7 +53176,7 @@
         <v>46058.796527777777</v>
       </c>
     </row>
-    <row r="404" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>1329</v>
       </c>
@@ -53243,7 +53250,7 @@
         <v>46008.442499999997</v>
       </c>
     </row>
-    <row r="405" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>485</v>
       </c>
@@ -53341,7 +53348,7 @@
         <v>46048.499305555553</v>
       </c>
     </row>
-    <row r="406" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>525</v>
       </c>
@@ -53433,7 +53440,7 @@
         <v>46048.734027777777</v>
       </c>
     </row>
-    <row r="407" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>530</v>
       </c>
@@ -53522,7 +53529,7 @@
         <v>46048.734027777777</v>
       </c>
     </row>
-    <row r="408" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>29</v>
       </c>
@@ -53617,7 +53624,7 @@
         <v>46058.800694444442</v>
       </c>
     </row>
-    <row r="409" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>24</v>
       </c>
@@ -53715,7 +53722,7 @@
         <v>46058.89166666667</v>
       </c>
     </row>
-    <row r="410" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>937</v>
       </c>
@@ -53813,7 +53820,7 @@
         <v>46055.999305555553</v>
       </c>
     </row>
-    <row r="411" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>458</v>
       </c>
@@ -53914,7 +53921,7 @@
         <v>46056.003472222219</v>
       </c>
     </row>
-    <row r="412" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>174</v>
       </c>
@@ -54009,7 +54016,7 @@
         <v>46067.711805555555</v>
       </c>
     </row>
-    <row r="413" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>233</v>
       </c>
@@ -54107,7 +54114,7 @@
         <v>46066.615277777775</v>
       </c>
     </row>
-    <row r="414" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>228</v>
       </c>
@@ -54205,7 +54212,7 @@
         <v>46066.615277777775</v>
       </c>
     </row>
-    <row r="415" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>513</v>
       </c>
@@ -54300,7 +54307,7 @@
         <v>46061.873611111114</v>
       </c>
     </row>
-    <row r="416" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>518</v>
       </c>
@@ -54389,7 +54396,7 @@
         <v>46061.873611111114</v>
       </c>
     </row>
-    <row r="417" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>453</v>
       </c>
@@ -54484,7 +54491,7 @@
         <v>46049.410416666666</v>
       </c>
     </row>
-    <row r="418" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>323</v>
       </c>
@@ -54582,7 +54589,7 @@
         <v>46050.788888888892</v>
       </c>
     </row>
-    <row r="419" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>102</v>
       </c>
@@ -54677,7 +54684,7 @@
         <v>46048.361111111109</v>
       </c>
     </row>
-    <row r="420" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>1250</v>
       </c>
@@ -54751,7 +54758,7 @@
         <v>46007.52138888889</v>
       </c>
     </row>
-    <row r="421" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>43</v>
       </c>
@@ -54849,7 +54856,7 @@
         <v>46048.560416666667</v>
       </c>
     </row>
-    <row r="422" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>598</v>
       </c>
@@ -54944,7 +54951,7 @@
         <v>46054.265277777777</v>
       </c>
     </row>
-    <row r="423" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>603</v>
       </c>
@@ -55039,7 +55046,7 @@
         <v>46067.709722222222</v>
       </c>
     </row>
-    <row r="424" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>1232</v>
       </c>
@@ -55113,7 +55120,7 @@
         <v>46007.492685185185</v>
       </c>
     </row>
-    <row r="425" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>1223</v>
       </c>
@@ -55187,7 +55194,7 @@
         <v>46007.435659722221</v>
       </c>
     </row>
-    <row r="426" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>1221</v>
       </c>
@@ -55264,7 +55271,7 @@
         <v>46007.435659722221</v>
       </c>
     </row>
-    <row r="427" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>555</v>
       </c>
@@ -55362,7 +55369,7 @@
         <v>46062.970138888886</v>
       </c>
     </row>
-    <row r="428" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>550</v>
       </c>
@@ -55460,7 +55467,7 @@
         <v>46059.527777777781</v>
       </c>
     </row>
-    <row r="429" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>348</v>
       </c>
@@ -55558,7 +55565,7 @@
         <v>46059.498611111114</v>
       </c>
     </row>
-    <row r="430" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>353</v>
       </c>
@@ -55653,7 +55660,7 @@
         <v>46059.498611111114</v>
       </c>
     </row>
-    <row r="431" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>261</v>
       </c>
@@ -55751,7 +55758,7 @@
         <v>46055.786111111112</v>
       </c>
     </row>
-    <row r="432" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>256</v>
       </c>
@@ -55849,7 +55856,7 @@
         <v>46055.78402777778</v>
       </c>
     </row>
-    <row r="433" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>646</v>
       </c>
@@ -55947,7 +55954,7 @@
         <v>46049.027083333334</v>
       </c>
     </row>
-    <row r="434" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>651</v>
       </c>
@@ -56045,7 +56052,7 @@
         <v>46048.920138888891</v>
       </c>
     </row>
-    <row r="435" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>569</v>
       </c>
@@ -56143,7 +56150,7 @@
         <v>46058.214583333334</v>
       </c>
     </row>
-    <row r="436" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>972</v>
       </c>
@@ -56241,7 +56248,7 @@
         <v>46058.186805555553</v>
       </c>
     </row>
-    <row r="437" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>944</v>
       </c>
@@ -56336,7 +56343,7 @@
         <v>46059.700694444444</v>
       </c>
     </row>
-    <row r="438" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>490</v>
       </c>
@@ -56428,7 +56435,7 @@
         <v>46059.700694444444</v>
       </c>
     </row>
-    <row r="439" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>898</v>
       </c>
@@ -56523,7 +56530,7 @@
         <v>46060.911111111112</v>
       </c>
     </row>
-    <row r="440" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>338</v>
       </c>
@@ -56621,7 +56628,7 @@
         <v>46062.010416666664</v>
       </c>
     </row>
-    <row r="441" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>664</v>
       </c>
@@ -56719,7 +56726,7 @@
         <v>46060.927083333336</v>
       </c>
     </row>
-    <row r="442" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>1156</v>
       </c>
@@ -56793,7 +56800,7 @@
         <v>46006.903124999997</v>
       </c>
     </row>
-    <row r="443" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>107</v>
       </c>
@@ -56894,7 +56901,7 @@
         <v>46067.711805555555</v>
       </c>
     </row>
-    <row r="444" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>112</v>
       </c>
@@ -56995,7 +57002,7 @@
         <v>46067.708333333336</v>
       </c>
     </row>
-    <row r="445" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>804</v>
       </c>
@@ -57093,7 +57100,7 @@
         <v>46050.742361111108</v>
       </c>
     </row>
-    <row r="446" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>1138</v>
       </c>
@@ -57167,7 +57174,7 @@
         <v>46001.368715277778</v>
       </c>
     </row>
-    <row r="447" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>126</v>
       </c>
@@ -57193,7 +57200,7 @@
         <v>46059.932638888888</v>
       </c>
     </row>
-    <row r="448" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>1123</v>
       </c>
@@ -57201,7 +57208,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="449" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>1121</v>
       </c>
@@ -57248,7 +57255,7 @@
         <v>46055.95045138889</v>
       </c>
     </row>
-    <row r="450" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>1118</v>
       </c>
@@ -57295,7 +57302,7 @@
         <v>46055.948287037034</v>
       </c>
     </row>
-    <row r="451" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>1115</v>
       </c>
@@ -57342,7 +57349,7 @@
         <v>46055.947268518517</v>
       </c>
     </row>
-    <row r="452" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>1112</v>
       </c>
@@ -57389,7 +57396,7 @@
         <v>46055.946168981478</v>
       </c>
     </row>
-    <row r="453" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>1103</v>
       </c>
@@ -57400,7 +57407,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="454" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>1101</v>
       </c>
@@ -57411,7 +57418,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="455" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>1098</v>
       </c>
@@ -57422,7 +57429,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="456" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>1096</v>
       </c>
@@ -57433,7 +57440,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="457" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>1093</v>
       </c>
@@ -57445,6 +57452,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AM457" xr:uid="{A7FE1BF5-4620-9740-887F-71B14DF2DAE5}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Celebrado"/>
+        <filter val="Ebrada"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>